<commit_message>
eliminación de duplicados y solucionados nan
</commit_message>
<xml_diff>
--- a/script_master_data_beltran/ficherosExcelOrigen/DED-AceleracionBacklog_Adopcion IA_v2a.xlsx
+++ b/script_master_data_beltran/ficherosExcelOrigen/DED-AceleracionBacklog_Adopcion IA_v2a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\6003305\Documents\tarea\estimacionIA_jdk21\script_master_data_beltran\ficherosExcelOrigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B455ED3E-36C0-430B-86B6-FFD9D9BBF31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59952DB1-6DB0-4914-87B5-DD2D4EB019F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-16125" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdopcionIA" sheetId="1" r:id="rId1"/>
@@ -2232,11 +2232,20 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2247,15 +2256,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3022,7 +3022,7 @@
   <dimension ref="B1:BR178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="AI6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="AI69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="AS5" sqref="AS5"/>
@@ -3352,7 +3352,7 @@
         <v>S</v>
       </c>
       <c r="AR6" s="28" t="str">
-        <f t="shared" ref="AR6:AS37" si="1">IF(OR(H6="S",M6="S",R6="S",W6="S",AB6="S",AG6="S",AL6="S"),"S","N")</f>
+        <f t="shared" ref="AR6:AR37" si="1">IF(OR(H6="S",M6="S",R6="S",W6="S",AB6="S",AG6="S",AL6="S"),"S","N")</f>
         <v>S</v>
       </c>
       <c r="AS6" s="180" t="s">
@@ -14512,7 +14512,7 @@
     </row>
     <row r="48" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="49" spans="3:66" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="193" t="s">
+      <c r="D49" s="186" t="s">
         <v>269</v>
       </c>
       <c r="E49" s="187"/>
@@ -14521,7 +14521,7 @@
       <c r="H49" s="187"/>
       <c r="I49" s="187"/>
       <c r="J49" s="188"/>
-      <c r="K49" s="186" t="s">
+      <c r="K49" s="191" t="s">
         <v>270</v>
       </c>
       <c r="L49" s="187"/>
@@ -14531,7 +14531,7 @@
       <c r="P49" s="187"/>
       <c r="Q49" s="187"/>
       <c r="R49" s="188"/>
-      <c r="S49" s="189" t="s">
+      <c r="S49" s="192" t="s">
         <v>271</v>
       </c>
       <c r="T49" s="187"/>
@@ -14541,7 +14541,7 @@
       <c r="X49" s="187"/>
       <c r="Y49" s="187"/>
       <c r="Z49" s="188"/>
-      <c r="AA49" s="190" t="s">
+      <c r="AA49" s="193" t="s">
         <v>272</v>
       </c>
       <c r="AB49" s="187"/>
@@ -14551,7 +14551,7 @@
       <c r="AF49" s="187"/>
       <c r="AG49" s="187"/>
       <c r="AH49" s="188"/>
-      <c r="AI49" s="194" t="s">
+      <c r="AI49" s="189" t="s">
         <v>273</v>
       </c>
       <c r="AJ49" s="187"/>
@@ -14561,7 +14561,7 @@
       <c r="AN49" s="187"/>
       <c r="AO49" s="187"/>
       <c r="AP49" s="188"/>
-      <c r="AQ49" s="195" t="s">
+      <c r="AQ49" s="190" t="s">
         <v>274</v>
       </c>
       <c r="AR49" s="187"/>
@@ -14571,7 +14571,7 @@
       <c r="AV49" s="187"/>
       <c r="AW49" s="187"/>
       <c r="AX49" s="188"/>
-      <c r="AY49" s="192" t="s">
+      <c r="AY49" s="195" t="s">
         <v>275</v>
       </c>
       <c r="AZ49" s="187"/>
@@ -14581,7 +14581,7 @@
       <c r="BD49" s="187"/>
       <c r="BE49" s="187"/>
       <c r="BF49" s="188"/>
-      <c r="BG49" s="191" t="s">
+      <c r="BG49" s="194" t="s">
         <v>276</v>
       </c>
       <c r="BH49" s="187"/>
@@ -16684,14 +16684,14 @@
     <row r="81" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="BG49:BN49"/>
+    <mergeCell ref="AY49:BF49"/>
     <mergeCell ref="D49:J49"/>
     <mergeCell ref="AI49:AP49"/>
     <mergeCell ref="AQ49:AX49"/>
     <mergeCell ref="K49:R49"/>
     <mergeCell ref="S49:Z49"/>
     <mergeCell ref="AA49:AH49"/>
-    <mergeCell ref="BG49:BN49"/>
-    <mergeCell ref="AY49:BF49"/>
   </mergeCells>
   <conditionalFormatting sqref="F51:F57">
     <cfRule type="dataBar" priority="9">

</xml_diff>

<commit_message>
Modificación en los prompts de los excels y corrección en el script para que tome desde la fila correcta los valores de las columnas
</commit_message>
<xml_diff>
--- a/script_master_data_beltran/ficherosExcelOrigen/DED-AceleracionBacklog_Adopcion IA_v2a.xlsx
+++ b/script_master_data_beltran/ficherosExcelOrigen/DED-AceleracionBacklog_Adopcion IA_v2a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\6003305\Documents\tarea\estimacionIA_jdk21\script_master_data_beltran\ficherosExcelOrigen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59952DB1-6DB0-4914-87B5-DD2D4EB019F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E8E47A-7ED3-4F0A-8EA2-50CCF444AC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -952,6 +952,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1032,18 +1033,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2232,11 +2234,17 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2250,12 +2258,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3022,10 +3024,10 @@
   <dimension ref="B1:BR178"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="5" topLeftCell="AI69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="5" topLeftCell="AN6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AS5" sqref="AS5"/>
+      <selection pane="bottomRight" activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14512,7 +14514,7 @@
     </row>
     <row r="48" spans="2:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="49" spans="3:66" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="186" t="s">
+      <c r="D49" s="190" t="s">
         <v>269</v>
       </c>
       <c r="E49" s="187"/>
@@ -14521,7 +14523,7 @@
       <c r="H49" s="187"/>
       <c r="I49" s="187"/>
       <c r="J49" s="188"/>
-      <c r="K49" s="191" t="s">
+      <c r="K49" s="193" t="s">
         <v>270</v>
       </c>
       <c r="L49" s="187"/>
@@ -14531,7 +14533,7 @@
       <c r="P49" s="187"/>
       <c r="Q49" s="187"/>
       <c r="R49" s="188"/>
-      <c r="S49" s="192" t="s">
+      <c r="S49" s="194" t="s">
         <v>271</v>
       </c>
       <c r="T49" s="187"/>
@@ -14541,7 +14543,7 @@
       <c r="X49" s="187"/>
       <c r="Y49" s="187"/>
       <c r="Z49" s="188"/>
-      <c r="AA49" s="193" t="s">
+      <c r="AA49" s="195" t="s">
         <v>272</v>
       </c>
       <c r="AB49" s="187"/>
@@ -14551,7 +14553,7 @@
       <c r="AF49" s="187"/>
       <c r="AG49" s="187"/>
       <c r="AH49" s="188"/>
-      <c r="AI49" s="189" t="s">
+      <c r="AI49" s="191" t="s">
         <v>273</v>
       </c>
       <c r="AJ49" s="187"/>
@@ -14561,7 +14563,7 @@
       <c r="AN49" s="187"/>
       <c r="AO49" s="187"/>
       <c r="AP49" s="188"/>
-      <c r="AQ49" s="190" t="s">
+      <c r="AQ49" s="192" t="s">
         <v>274</v>
       </c>
       <c r="AR49" s="187"/>
@@ -14571,7 +14573,7 @@
       <c r="AV49" s="187"/>
       <c r="AW49" s="187"/>
       <c r="AX49" s="188"/>
-      <c r="AY49" s="195" t="s">
+      <c r="AY49" s="189" t="s">
         <v>275</v>
       </c>
       <c r="AZ49" s="187"/>
@@ -14581,7 +14583,7 @@
       <c r="BD49" s="187"/>
       <c r="BE49" s="187"/>
       <c r="BF49" s="188"/>
-      <c r="BG49" s="194" t="s">
+      <c r="BG49" s="186" t="s">
         <v>276</v>
       </c>
       <c r="BH49" s="187"/>

</xml_diff>